<commit_message>
Added trigger to database to auto update lastmodifieddate on Mim records. Added a new bug to Todo
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -122,6 +122,9 @@
   <si>
     <t>20ec569141f8e3e7cc826ccdc5f32f445c933915</t>
   </si>
+  <si>
+    <t>Continue this Mimry is not working properly because of the recent Required Creator field</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +193,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{83701CBD-8807-4348-88C6-E4A90E042701}" diskRevisions="1" revisionId="7" version="3">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5B619EE2-1192-40BD-B54E-DBAAAB4ED313}" diskRevisions="1" revisionId="19" version="5">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -204,6 +207,18 @@
     </sheetIdMap>
   </header>
   <header guid="{83701CBD-8807-4348-88C6-E4A90E042701}" dateTime="2014-04-16T14:34:20" maxSheetId="3" userName="Luong Hoang" r:id="rId3" minRId="4" maxRId="6">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E371FB39-50EE-4703-9547-B1A2268D2A1E}" dateTime="2014-04-16T19:52:09" maxSheetId="3" userName="Luong Hoang" r:id="rId4" minRId="8" maxRId="17">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5B619EE2-1192-40BD-B54E-DBAAAB4ED313}" dateTime="2014-04-16T19:53:05" maxSheetId="3" userName="Luong Hoang" r:id="rId5">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -264,6 +279,98 @@
       </is>
     </nc>
   </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="8" sId="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Continue this Mimry is not working properly because of the recent Required Creator field</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="1">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>1 - Urgent</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="10" sId="1">
+    <nc r="F2" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" sId="1">
+    <nc r="F5" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="12" sId="1">
+    <nc r="F6" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" sId="1">
+    <nc r="F9" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="1">
+    <nc r="F10" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="15" sId="1">
+    <nc r="F11" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="1">
+    <nc r="F12" t="inlineStr">
+      <is>
+        <t>Open</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="17" sId="1">
+    <nc r="F13" t="inlineStr">
+      <is>
+        <t>In Progress</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
   <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Sheet1!$A$1:$F$2000</formula>
@@ -544,7 +651,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +660,7 @@
     <col min="3" max="3" width="106" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -577,13 +685,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -622,24 +733,30 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -659,7 +776,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -681,51 +798,72 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -12166,22 +12304,28 @@
   </sheetData>
   <autoFilter ref="A1:F2000">
     <filterColumn colId="5">
-      <filters blank="1"/>
+      <filters blank="1">
+        <filter val="In Progress"/>
+        <filter val="Open"/>
+      </filters>
     </filterColumn>
-    <sortState ref="A2:F2000">
+    <sortState ref="A2:F13">
       <sortCondition ref="B1:B2000"/>
     </sortState>
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C14" sqref="C14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
         <filterColumn colId="5">
-          <filters blank="1"/>
+          <filters blank="1">
+            <filter val="In Progress"/>
+            <filter val="Open"/>
+          </filters>
         </filterColumn>
-        <sortState ref="A2:F2000">
+        <sortState ref="A2:F13">
           <sortCondition ref="B1:B2000"/>
         </sortState>
       </autoFilter>
@@ -12256,4 +12400,19 @@
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
+  <rowSortMap ref="A2:XFD13" count="8">
+    <row newVal="1" oldVal="12"/>
+    <row newVal="4" oldVal="1"/>
+    <row newVal="5" oldVal="4"/>
+    <row newVal="8" oldVal="5"/>
+    <row newVal="9" oldVal="8"/>
+    <row newVal="10" oldVal="9"/>
+    <row newVal="11" oldVal="10"/>
+    <row newVal="12" oldVal="11"/>
+  </rowSortMap>
+</worksheetSortMap>
 </file>
</xml_diff>

<commit_message>
- Add more sql triggers - Updated todo
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Websites\Mimry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhoang\Documents\Git\Mimry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1616" windowHeight="876" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -125,6 +125,9 @@
   <si>
     <t>Continue this Mimry is not working properly because of the recent Required Creator field</t>
   </si>
+  <si>
+    <t>Look into custom validation for Image field</t>
+  </si>
 </sst>
 </file>
 
@@ -193,7 +196,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5B619EE2-1192-40BD-B54E-DBAAAB4ED313}" diskRevisions="1" revisionId="19" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{91D58D56-3D84-4D0F-9A4D-F70871E82F7E}" diskRevisions="1" revisionId="22" version="6">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -219,6 +222,12 @@
     </sheetIdMap>
   </header>
   <header guid="{5B619EE2-1192-40BD-B54E-DBAAAB4ED313}" dateTime="2014-04-16T19:53:05" maxSheetId="3" userName="Luong Hoang" r:id="rId5">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{91D58D56-3D84-4D0F-9A4D-F70871E82F7E}" dateTime="2014-04-16T23:35:36" maxSheetId="3" userName="Luong Hoang" r:id="rId6" minRId="20" maxRId="21">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -371,6 +380,31 @@
 
 <file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="20" sId="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Look into custom validation for Image field</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" sId="1">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>2 - Important</t>
+      </is>
+    </nc>
+  </rcc>
   <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
   <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
     <formula>Sheet1!$A$1:$F$2000</formula>
@@ -651,7 +685,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,6 +904,12 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -12315,7 +12355,7 @@
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C12" sqref="C12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">

</xml_diff>

<commit_message>
- Changed view for Mimry index to use bootstrap grid fluid system. On   large devices display 4 mims on one row, medium shows 3, small shows 2   and extra small shows 1. - Updated todo
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Websites\Mimry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhoang\Documents\Git\Mimry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -170,6 +170,9 @@
   <si>
     <t>Redesign home page Mimry index view to wrap Mims around full-width page.</t>
   </si>
+  <si>
+    <t>Display Mimries ordered by most recent modified date</t>
+  </si>
 </sst>
 </file>
 
@@ -244,7 +247,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C520CB6E-3B84-4143-97B8-C6B963A18411}" diskRevisions="1" revisionId="54" version="11">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{63A805DB-396E-4F6F-BB79-4A07C829A5EC}" diskRevisions="1" revisionId="57" version="12">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -306,6 +309,12 @@
     </sheetIdMap>
   </header>
   <header guid="{C520CB6E-3B84-4143-97B8-C6B963A18411}" dateTime="2014-04-20T17:20:06" maxSheetId="3" userName="Luong Hoang" r:id="rId11" minRId="52" maxRId="53">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{63A805DB-396E-4F6F-BB79-4A07C829A5EC}" dateTime="2014-04-21T13:47:24" maxSheetId="3" userName="Luong Hoang" r:id="rId12" minRId="55" maxRId="56">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -419,6 +428,31 @@
     <nc r="C20" t="inlineStr">
       <is>
         <t>Redesign home page Mimry index view to wrap Mims around full-width page.</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="55" sId="1">
+    <nc r="B21" t="inlineStr">
+      <is>
+        <t>2 - Important</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="56" sId="1">
+    <nc r="C21" t="inlineStr">
+      <is>
+        <t>Display Mimries ordered by most recent modified date</t>
       </is>
     </nc>
   </rcc>
@@ -805,7 +839,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{63A805DB-396E-4F6F-BB79-4A07C829A5EC}" name="Luong Hoang" id="-948929620" dateTime="2014-04-21T12:22:38"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,7 +1111,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,27 +1410,24 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>22</v>
@@ -1402,7 +1435,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -12813,7 +12855,7 @@
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
@@ -12901,7 +12943,7 @@
 
 <file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
-  <rowSortMap ref="A3:XFD20" count="18">
+  <rowSortMap ref="A3:XFD21" count="19">
     <row newVal="2" oldVal="5"/>
     <row newVal="3" oldVal="13"/>
     <row newVal="4" oldVal="14"/>
@@ -12918,8 +12960,9 @@
     <row newVal="15" oldVal="9"/>
     <row newVal="16" oldVal="18"/>
     <row newVal="17" oldVal="19"/>
-    <row newVal="18" oldVal="10"/>
-    <row newVal="19" oldVal="11"/>
+    <row newVal="18" oldVal="20"/>
+    <row newVal="19" oldVal="10"/>
+    <row newVal="20" oldVal="11"/>
   </rowSortMap>
 </worksheetSortMap>
 </file>
</xml_diff>

<commit_message>
Added ability to unvote
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1176" activeSheetId="1"/>
+    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -209,6 +209,9 @@
   <si>
     <t>Add ability for users to upload image from computer when creating/editing image</t>
   </si>
+  <si>
+    <t xml:space="preserve">Add global error panel to display whenever some action fails, especially ajax post </t>
+  </si>
 </sst>
 </file>
 
@@ -260,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,6 +279,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -296,7 +302,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F6A2C815-D5AF-4077-93EC-81CDF5014EC8}" diskRevisions="1" revisionId="93" version="20">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AE18EE4E-38AA-44AE-B5C6-C9BB5A67915E}" diskRevisions="1" revisionId="96" version="21">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -412,6 +418,12 @@
     </sheetIdMap>
   </header>
   <header guid="{F6A2C815-D5AF-4077-93EC-81CDF5014EC8}" dateTime="2014-04-30T17:49:22" maxSheetId="3" userName="Luong Hoang" r:id="rId20" minRId="91" maxRId="92">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AE18EE4E-38AA-44AE-B5C6-C9BB5A67915E}" dateTime="2014-05-03T01:36:31" maxSheetId="3" userName="Luong Hoang" r:id="rId21" minRId="94" maxRId="95">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -899,6 +911,31 @@
     <nc r="C32" t="inlineStr">
       <is>
         <t>Add ability for users to upload image from computer when creating/editing image</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="94" sId="1">
+    <nc r="C33" t="inlineStr">
+      <is>
+        <t xml:space="preserve">Add global error panel to display whenever some action fails, especially ajax post </t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="95" sId="1">
+    <nc r="B33" t="inlineStr">
+      <is>
+        <t>1 - Urgent</t>
       </is>
     </nc>
   </rcc>
@@ -1532,7 +1569,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,16 +1670,13 @@
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -1792,13 +1826,13 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>21</v>
@@ -1806,13 +1840,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1834,243 +1871,249 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>39</v>
+      <c r="C19" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>21</v>
+      <c r="C20" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -13348,7 +13391,7 @@
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C27" sqref="C27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
@@ -13436,13 +13479,13 @@
 
 <file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
-  <rowSortMap ref="A2:XFD32" count="30">
+  <rowSortMap ref="A2:XFD33" count="30">
     <row newVal="1" oldVal="22"/>
     <row newVal="2" oldVal="23"/>
     <row newVal="3" oldVal="13"/>
     <row newVal="4" oldVal="14"/>
     <row newVal="5" oldVal="25"/>
-    <row newVal="6" oldVal="1"/>
+    <row newVal="6" oldVal="32"/>
     <row newVal="7" oldVal="12"/>
     <row newVal="8" oldVal="4"/>
     <row newVal="9" oldVal="2"/>
@@ -13451,22 +13494,22 @@
     <row newVal="12" oldVal="7"/>
     <row newVal="13" oldVal="8"/>
     <row newVal="14" oldVal="15"/>
-    <row newVal="15" oldVal="5"/>
+    <row newVal="15" oldVal="1"/>
+    <row newVal="16" oldVal="5"/>
     <row newVal="17" oldVal="19"/>
-    <row newVal="18" oldVal="17"/>
-    <row newVal="19" oldVal="9"/>
-    <row newVal="20" oldVal="18"/>
-    <row newVal="21" oldVal="20"/>
-    <row newVal="22" oldVal="21"/>
-    <row newVal="23" oldVal="24"/>
-    <row newVal="24" oldVal="26"/>
-    <row newVal="25" oldVal="27"/>
-    <row newVal="26" oldVal="28"/>
-    <row newVal="27" oldVal="29"/>
-    <row newVal="28" oldVal="31"/>
-    <row newVal="29" oldVal="30"/>
-    <row newVal="30" oldVal="10"/>
-    <row newVal="31" oldVal="11"/>
+    <row newVal="18" oldVal="16"/>
+    <row newVal="19" oldVal="17"/>
+    <row newVal="20" oldVal="9"/>
+    <row newVal="21" oldVal="18"/>
+    <row newVal="22" oldVal="20"/>
+    <row newVal="23" oldVal="21"/>
+    <row newVal="25" oldVal="26"/>
+    <row newVal="26" oldVal="27"/>
+    <row newVal="27" oldVal="28"/>
+    <row newVal="28" oldVal="29"/>
+    <row newVal="29" oldVal="31"/>
+    <row newVal="31" oldVal="10"/>
+    <row newVal="32" oldVal="11"/>
   </rowSortMap>
 </worksheetSortMap>
 </file>
</xml_diff>

<commit_message>
Fixed UI bug where unliking/unvoting doesn't change the style properly in IE
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -221,6 +221,12 @@
   <si>
     <t>Changed icons for facebook/google/twtr login</t>
   </si>
+  <si>
+    <t xml:space="preserve">Unliking or Unvoting doesn't change icon color properly in IE </t>
+  </si>
+  <si>
+    <t>Changed css to remove active,focus style of anchor element</t>
+  </si>
 </sst>
 </file>
 
@@ -311,7 +317,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{EDCE4133-4786-4967-915C-54A1E2E25CC3}" diskRevisions="1" revisionId="106" version="25">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AD2362F7-F20A-4AF7-BA63-2AD50A6A9A74}" diskRevisions="1" revisionId="112" version="27">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -457,6 +463,18 @@
     </sheetIdMap>
   </header>
   <header guid="{EDCE4133-4786-4967-915C-54A1E2E25CC3}" dateTime="2014-05-03T12:52:07" maxSheetId="3" userName="Luong Hoang" r:id="rId25" minRId="104" maxRId="105">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{25E7BC9D-B724-4950-8347-5D6A5CECD514}" dateTime="2014-05-03T13:00:00" maxSheetId="3" userName="Luong Hoang" r:id="rId26" minRId="107" maxRId="108">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AD2362F7-F20A-4AF7-BA63-2AD50A6A9A74}" dateTime="2014-05-03T13:06:28" maxSheetId="3" userName="Luong Hoang" r:id="rId27" minRId="110" maxRId="111">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1055,6 +1073,56 @@
     <nc r="B35" t="inlineStr">
       <is>
         <t>2 - Important</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="107" sId="1">
+    <nc r="C36" t="inlineStr">
+      <is>
+        <t xml:space="preserve">Unliking or Unvoting doesn't change icon color properly in IE </t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="108" sId="1">
+    <nc r="B36" t="inlineStr">
+      <is>
+        <t>3 - Nice to have</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="110" sId="1">
+    <nc r="F36" t="inlineStr">
+      <is>
+        <t>Closed</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="111" sId="1">
+    <nc r="D36" t="inlineStr">
+      <is>
+        <t>Changed css to remove active,focus style of anchor element</t>
       </is>
     </nc>
   </rcc>
@@ -1688,7 +1756,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,9 +2258,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -13528,7 +13608,7 @@
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="A36" sqref="A36"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">

</xml_diff>

<commit_message>
- Modified css for textarea so that it spans 100% width. This is used for   comment box - Added placeholder comment textarea input control next to the Mimry   details. Current behavior is to stack to bottom if page is resized to small   devices. - Added view mode to partial view Mim to display in thumbnail mode or full   mode.
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -230,6 +230,9 @@
   <si>
     <t>Add ability to share a Mimry or a Mim to social sites such as FB, Twtr</t>
   </si>
+  <si>
+    <t>Add captcha to user registration</t>
+  </si>
 </sst>
 </file>
 
@@ -320,7 +323,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B75D6E66-A6FA-4C96-915D-B1BC88D67023}" diskRevisions="1" revisionId="115" version="28">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1D239E26-2FA6-410E-AFC5-FCFD21DD18FD}" diskRevisions="1" revisionId="118" version="29">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -484,6 +487,12 @@
     </sheetIdMap>
   </header>
   <header guid="{B75D6E66-A6FA-4C96-915D-B1BC88D67023}" dateTime="2014-05-03T13:12:39" maxSheetId="3" userName="Luong Hoang" r:id="rId28" minRId="113" maxRId="114">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1D239E26-2FA6-410E-AFC5-FCFD21DD18FD}" dateTime="2014-05-03T14:05:20" maxSheetId="3" userName="Luong Hoang" r:id="rId29" minRId="116" maxRId="117">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1169,6 +1178,31 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="116" sId="1">
+    <nc r="C38" t="inlineStr">
+      <is>
+        <t>Add captcha to user registration</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="117" sId="1">
+    <nc r="B38" t="inlineStr">
+      <is>
+        <t>2 - Important</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="4" sId="1">
@@ -1790,7 +1824,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2255,38 +2289,35 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>54</v>
+        <v>6</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>63</v>
+      <c r="C34" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2308,13 +2339,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>21</v>
@@ -2322,7 +2353,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>11</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -13648,7 +13688,7 @@
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B38" sqref="B38"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
@@ -13736,7 +13776,7 @@
 
 <file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
-  <rowSortMap ref="A2:XFD37" count="31">
+  <rowSortMap ref="A2:XFD38" count="32">
     <row newVal="1" oldVal="22"/>
     <row newVal="2" oldVal="23"/>
     <row newVal="3" oldVal="13"/>
@@ -13764,10 +13804,11 @@
     <row newVal="25" oldVal="24"/>
     <row newVal="30" oldVal="31"/>
     <row newVal="31" oldVal="34"/>
-    <row newVal="32" oldVal="30"/>
-    <row newVal="33" oldVal="36"/>
-    <row newVal="34" oldVal="10"/>
-    <row newVal="36" oldVal="11"/>
+    <row newVal="32" oldVal="37"/>
+    <row newVal="33" oldVal="30"/>
+    <row newVal="34" oldVal="36"/>
+    <row newVal="36" oldVal="10"/>
+    <row newVal="37" oldVal="11"/>
   </rowSortMap>
 </worksheetSortMap>
 </file>
</xml_diff>

<commit_message>
- Added models for Comment, Comment Likes and Comment Votes - Added migration for new model changes - Hooked up UI to Actions for posting and viewing comments using ajax post   with anti forgery token - Refactored base interface model such as IDateCreated to IUserAction to   automatically include User value as well - Added unobtrusive jquery ajax files to handle ajax update of form   controls
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -233,6 +233,9 @@
   <si>
     <t>Add captcha to user registration</t>
   </si>
+  <si>
+    <t>Handle posting comments that contain scripts or dangerous scripts</t>
+  </si>
 </sst>
 </file>
 
@@ -323,7 +326,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1D239E26-2FA6-410E-AFC5-FCFD21DD18FD}" diskRevisions="1" revisionId="118" version="29">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7250EBEC-39A1-49F1-B573-617D0B8129E1}" diskRevisions="1" revisionId="121" version="30">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -493,6 +496,12 @@
     </sheetIdMap>
   </header>
   <header guid="{1D239E26-2FA6-410E-AFC5-FCFD21DD18FD}" dateTime="2014-05-03T14:05:20" maxSheetId="3" userName="Luong Hoang" r:id="rId29" minRId="116" maxRId="117">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7250EBEC-39A1-49F1-B573-617D0B8129E1}" dateTime="2014-05-08T00:42:41" maxSheetId="3" userName="Luong Hoang" r:id="rId30" minRId="119" maxRId="120">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1235,6 +1244,31 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="119" sId="1">
+    <nc r="C39" t="inlineStr">
+      <is>
+        <t>Handle posting comments that contain scripts or dangerous scripts</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="120" sId="1">
+    <nc r="B39" t="inlineStr">
+      <is>
+        <t>2 - Important</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="8" sId="1">
@@ -1823,8 +1857,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,24 +2334,24 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>54</v>
+        <v>6</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>63</v>
+      <c r="C35" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2339,27 +2373,24 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>21</v>
@@ -2367,7 +2398,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>11</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -13687,8 +13727,8 @@
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="B38" sqref="B38"/>
+    <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1" topLeftCell="A6">
+      <selection activeCell="C22" sqref="C22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
@@ -13776,7 +13816,7 @@
 
 <file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
-  <rowSortMap ref="A2:XFD38" count="32">
+  <rowSortMap ref="A2:XFD39" count="32">
     <row newVal="1" oldVal="22"/>
     <row newVal="2" oldVal="23"/>
     <row newVal="3" oldVal="13"/>
@@ -13805,10 +13845,10 @@
     <row newVal="30" oldVal="31"/>
     <row newVal="31" oldVal="34"/>
     <row newVal="32" oldVal="37"/>
-    <row newVal="33" oldVal="30"/>
-    <row newVal="34" oldVal="36"/>
-    <row newVal="36" oldVal="10"/>
-    <row newVal="37" oldVal="11"/>
+    <row newVal="33" oldVal="38"/>
+    <row newVal="34" oldVal="30"/>
+    <row newVal="37" oldVal="10"/>
+    <row newVal="38" oldVal="11"/>
   </rowSortMap>
 </worksheetSortMap>
 </file>
</xml_diff>

<commit_message>
Added comment count and like count display
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -236,6 +236,9 @@
   <si>
     <t>Handle posting comments that contain scripts or dangerous scripts</t>
   </si>
+  <si>
+    <t>Added commenting on mimries</t>
+  </si>
 </sst>
 </file>
 
@@ -326,7 +329,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7250EBEC-39A1-49F1-B573-617D0B8129E1}" diskRevisions="1" revisionId="121" version="30">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{7E5BE945-9025-471B-85E0-12EB60365244}" diskRevisions="1" revisionId="124" version="31">
   <header guid="{CA7B1163-FA92-4C5A-A594-515B3F00B4D8}" dateTime="2014-04-15T16:09:52" maxSheetId="3" userName="Luong Hoang" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -502,6 +505,12 @@
     </sheetIdMap>
   </header>
   <header guid="{7250EBEC-39A1-49F1-B573-617D0B8129E1}" dateTime="2014-05-08T00:42:41" maxSheetId="3" userName="Luong Hoang" r:id="rId30" minRId="119" maxRId="120">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7E5BE945-9025-471B-85E0-12EB60365244}" dateTime="2014-05-08T23:20:22" maxSheetId="3" userName="Luong Hoang" r:id="rId31" minRId="122" maxRId="123">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1269,6 +1278,31 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="122" sId="1">
+    <nc r="D24" t="inlineStr">
+      <is>
+        <t>Added commenting on mimries</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="123" sId="1">
+    <nc r="F24" t="inlineStr">
+      <is>
+        <t>Closed</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="8" sId="1">
@@ -1857,8 +1891,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F2000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,7 +1941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>23</v>
       </c>
@@ -1916,6 +1950,12 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>47</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -13722,13 +13762,13 @@
         <customFilter operator="notEqual" val="*closed*"/>
       </customFilters>
     </filterColumn>
-    <sortState ref="A3:F2000">
+    <sortState ref="A6:F2000">
       <sortCondition ref="B2:B2000"/>
     </sortState>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1" topLeftCell="A6">
-      <selection activeCell="C22" sqref="C22"/>
+    <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
+      <selection activeCell="C26" sqref="C26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
@@ -13737,7 +13777,7 @@
             <customFilter operator="notEqual" val="*closed*"/>
           </customFilters>
         </filterColumn>
-        <sortState ref="A3:F2000">
+        <sortState ref="A6:F2000">
           <sortCondition ref="B2:B2000"/>
         </sortState>
       </autoFilter>

</xml_diff>

<commit_message>
Added code to delete Mimry altogther if user deletes the only Mim belonging to it. However, currently it's unknown whether deleting Mim is a good behavior to have. An issue was added to consider this more carefully.
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhoang\Documents\Git\Mimry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Websites\Mimry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <customWorkbookViews>
-    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1616" windowHeight="876" activeSheetId="1"/>
+    <customWorkbookView name="Luong Hoang - Personal View" guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1688" yWindow="-8" windowWidth="1696" windowHeight="1026" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -260,6 +260,9 @@
   <si>
     <t>Redesign Mim Delete &amp; Delete Confirm page</t>
   </si>
+  <si>
+    <t>Does it make sense to allow deleting of Mims? If so under what conditions should this be allowed? What if people have voted/commented on the mimry? Etc…</t>
+  </si>
 </sst>
 </file>
 
@@ -350,7 +353,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{664315EC-7047-4FFF-82D1-E5862A94B2D8}" diskRevisions="1" revisionId="143" version="36">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BF1B498E-1294-4D18-94B8-776FD1173264}" diskRevisions="1" revisionId="146" version="37">
   <header guid="{99B1F7B3-F860-489A-8962-33216AF0A170}" dateTime="2014-04-19T11:32:46" maxSheetId="3" userName="Luong Hoang" r:id="rId9" minRId="37" maxRId="40">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -514,6 +517,12 @@
     </sheetIdMap>
   </header>
   <header guid="{664315EC-7047-4FFF-82D1-E5862A94B2D8}" dateTime="2014-05-18T15:46:18" maxSheetId="3" userName="Luong Hoang" r:id="rId36" minRId="139" maxRId="142">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BF1B498E-1294-4D18-94B8-776FD1173264}" dateTime="2014-05-18T21:55:29" maxSheetId="3" userName="Luong Hoang" r:id="rId37" minRId="144" maxRId="145">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -988,6 +997,31 @@
         </bottom>
       </border>
     </ndxf>
+  </rcc>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Sheet1!$A$1:$F$2000</formula>
+    <oldFormula>Sheet1!$A$1:$F$2000</oldFormula>
+  </rdn>
+  <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="144" sId="1">
+    <nc r="C43" t="inlineStr">
+      <is>
+        <t>Does it make sense to allow deleting of Mims? If so under what conditions should this be allowed? What if people have voted/commented on the mimry? Etc…</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="145" sId="1">
+    <nc r="B43" t="inlineStr">
+      <is>
+        <t>4 - Minor Issue</t>
+      </is>
+    </nc>
   </rcc>
   <rcv guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" action="delete"/>
   <rdn rId="0" localSheetId="1" customView="1" name="Z_CAA0D881_FDF1_4DCC_8B08_F9ACA23031E2_.wvu.FilterData" hidden="1" oldHidden="1">
@@ -1715,7 +1749,7 @@
   <dimension ref="A1:F2000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,21 +2349,27 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -13630,7 +13670,7 @@
   </autoFilter>
   <customSheetViews>
     <customSheetView guid="{CAA0D881-FDF1-4DCC-8B08-F9ACA23031E2}" filter="1" showAutoFilter="1">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C32" sqref="C32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:F2000">
@@ -13718,7 +13758,7 @@
 
 <file path=xl/worksheets/wsSortMap1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheetSortMap xmlns="http://schemas.microsoft.com/office/excel/2006/main">
-  <rowSortMap ref="A2:XFD42" count="36">
+  <rowSortMap ref="A2:XFD43" count="37">
     <row newVal="1" oldVal="22"/>
     <row newVal="2" oldVal="23"/>
     <row newVal="3" oldVal="13"/>
@@ -13754,7 +13794,8 @@
     <row newVal="38" oldVal="30"/>
     <row newVal="39" oldVal="36"/>
     <row newVal="40" oldVal="10"/>
-    <row newVal="41" oldVal="11"/>
+    <row newVal="41" oldVal="42"/>
+    <row newVal="42" oldVal="11"/>
   </rowSortMap>
 </worksheetSortMap>
 </file>
</xml_diff>